<commit_message>
Add Department and Add Department Permission through Excel implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/AddDepartment.xlsx
+++ b/src/main/resources/AddDepartment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvenkata\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvenkata\intellij-workspace\Employee-Management-System\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B4654A-85BF-4E0F-8833-127995F743E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB0653-6DC3-4801-8E31-52017C2B8122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B793C1C-B26A-4716-8C9C-94173732327F}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{9B793C1C-B26A-4716-8C9C-94173732327F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>department_name</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Capita</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Add</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F39B44-1F15-477A-BA26-CC87B04F3B0A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,28 +434,37 @@
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>